<commit_message>
Research Data - 3001121619 업데이트
</commit_message>
<xml_diff>
--- a/Data/Research Data - 3001121619/3001121619.xlsx
+++ b/Data/Research Data - 3001121619/3001121619.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Program Files (x86)\Steam\steamapps\common\RimWorld\Mods\RMK\Data\Research Data - 3001121619\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bjmi0\Desktop\림월드 번역\Research Data - 3001121619\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D36C545-0984-498E-BCD8-BAA75BF8BB44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA58459F-2D3A-488A-9177-783A1E37B478}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main_240603" sheetId="1" r:id="rId1"/>
@@ -32,8 +32,70 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>bjmi0</author>
+  </authors>
+  <commentList>
+    <comment ref="E95" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>2025-01-07에 삭제됨. 삭제 이전 번역문: '연구자료'</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E96" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>2025-01-07에 삭제됨. 삭제 이전 번역문: '첨단 연구자료'</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E97" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>2025-01-07에 삭제됨. 삭제 이전 번역문: '암호화 연구자료'</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E99" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000004000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>2025-01-07에 새로 추가된 노드들 (3개)</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="486" uniqueCount="335">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="498" uniqueCount="344">
   <si>
     <t>Class+Node [(Identifier (Key)]</t>
   </si>
@@ -65,6 +127,9 @@
     <t>Bio. Schematics</t>
   </si>
   <si>
+    <t>자연과학 선행연구</t>
+  </si>
+  <si>
     <t>ThingDef+BiologySchematics.description</t>
   </si>
   <si>
@@ -74,6 +139,9 @@
     <t>Biology schematics are helpful when doing research, as they give a better research understanding for a time when read. They come in 3 types and stack with each other.\n\nSchematics works with the drug policy system but without any negative sides besides the cost, as they are expansive but can give a huge bonus to your research if stacked together.</t>
   </si>
   <si>
+    <t>사용 시 앞선 연구자들의 자연과학 선행연구를 검토하여 연구 진척이 빨라집니다. 선행연구는 세 가지 분야가 존재하며 각 분야의 선행연구 효과는 중첩할 수 있습니다.\n\n선행연구는 약물과 같은 방식으로 작동하지만 부작용이 존재하지 않으며, 중첩할수록 눈에 띄는 효과를 보입니다.</t>
+  </si>
+  <si>
     <t>ThingDef+BiologySchematics.ingestible.ingestCommandString</t>
   </si>
   <si>
@@ -83,6 +151,9 @@
     <t>Read {0}</t>
   </si>
   <si>
+    <t>{0} 검토하기</t>
+  </si>
+  <si>
     <t>ThingDef+BiologySchematics.ingestible.ingestReportString</t>
   </si>
   <si>
@@ -92,6 +163,9 @@
     <t>Reading {0}.</t>
   </si>
   <si>
+    <t>{0} 검토하는 중</t>
+  </si>
+  <si>
     <t>HediffDef+BiologySchematicsBonus.label</t>
   </si>
   <si>
@@ -104,6 +178,9 @@
     <t>Biology Schematics</t>
   </si>
   <si>
+    <t>자연과학 선행연구 검토</t>
+  </si>
+  <si>
     <t>HediffDef+BiologySchematicsBonus.labelNoun</t>
   </si>
   <si>
@@ -119,6 +196,9 @@
     <t>BiologySchematicsBonus.description</t>
   </si>
   <si>
+    <t>앞선 연구자들의 자연과학 선행연구를 검토하여 연구 진척이 빨라집니다. 선행연구는 세 가지 분야가 존재하며 각 분야의 선행연구 효과는 중첩할 수 있습니다.\n\n선행연구는 약물과 같은 방식으로 작동하지만 부작용이 존재하지 않으며, 중첩할수록 눈에 띄는 효과를 보입니다.</t>
+  </si>
+  <si>
     <t>ThingDef+ClinicalSchematics.label</t>
   </si>
   <si>
@@ -128,6 +208,9 @@
     <t>Cli. Schematics</t>
   </si>
   <si>
+    <t>수리과학 선행연구</t>
+  </si>
+  <si>
     <t>ThingDef+ClinicalSchematics.description</t>
   </si>
   <si>
@@ -137,6 +220,9 @@
     <t>Clinical schematics are helpful when doing research, as they give a better research understanding for a time when read. They come in 3 types and stack with each other.\n\nSchematics works with the drug policy system but without any negative sides besides the cost, as they are expansive but can give a huge bonus to your research if stacked together.</t>
   </si>
   <si>
+    <t>사용 시 앞선 연구자들의 수리과학 선행연구를 검토하여 연구 진척이 빨라집니다. 선행연구는 세 가지 분야가 존재하며 각 분야의 선행연구 효과는 중첩할 수 있습니다.\n\n선행연구는 약물과 같은 방식으로 작동하지만 부작용이 존재하지 않으며, 중첩할수록 눈에 띄는 효과를 보입니다.</t>
+  </si>
+  <si>
     <t>ThingDef+ClinicalSchematics.ingestible.ingestCommandString</t>
   </si>
   <si>
@@ -158,6 +244,9 @@
     <t>Clinical Schematics</t>
   </si>
   <si>
+    <t>수리과학 선행연구 검토</t>
+  </si>
+  <si>
     <t>HediffDef+ClinicalSchematicsBonus.labelNoun</t>
   </si>
   <si>
@@ -173,6 +262,9 @@
     <t>ClinicalSchematicsBonus.description</t>
   </si>
   <si>
+    <t>앞선 연구자들의 수리과학 선행연구를 검토하여 연구 진척이 빨라집니다. 선행연구는 세 가지 분야가 존재하며 각 분야의 선행연구 효과는 중첩할 수 있습니다.\n\n선행연구는 약물과 같은 방식으로 작동하지만 부작용이 존재하지 않으며, 중첩할수록 눈에 띄는 효과를 보입니다.</t>
+  </si>
+  <si>
     <t>ThingDef+EngineeringSchematics.label</t>
   </si>
   <si>
@@ -182,6 +274,9 @@
     <t>Eng. Schematics</t>
   </si>
   <si>
+    <t>응용과학 선행연구</t>
+  </si>
+  <si>
     <t>ThingDef+EngineeringSchematics.description</t>
   </si>
   <si>
@@ -191,6 +286,9 @@
     <t>Engineering schematics are helpful when doing research, as they give a better research understanding for a time when read. They come in 3 types and stack with each other.\n\nSchematics works with the drug policy system but without any negative sides besides the cost, as they are expansive but can give a huge bonus to your research if stacked together.</t>
   </si>
   <si>
+    <t>사용 시 앞선 연구자들의 응용과학 선행연구를 검토하여 연구 진척이 빨라집니다. 선행연구는 세 가지 분야가 존재하며 각 분야의 선행연구 효과는 중첩할 수 있습니다.\n\n선행연구는 약물과 같은 방식으로 작동하지만 부작용이 존재하지 않으며, 중첩할수록 눈에 띄는 효과를 보입니다.</t>
+  </si>
+  <si>
     <t>ThingDef+EngineeringSchematics.ingestible.ingestCommandString</t>
   </si>
   <si>
@@ -212,6 +310,9 @@
     <t>Engineering Schematics</t>
   </si>
   <si>
+    <t>응용과학 선행연구 검토</t>
+  </si>
+  <si>
     <t>HediffDef+EngineeringSchematicsBonus.labelNoun</t>
   </si>
   <si>
@@ -227,6 +328,9 @@
     <t>EngineeringSchematicsBonus.description</t>
   </si>
   <si>
+    <t>앞선 연구자들의 응용과학 선행연구를 검토하여 연구 진척이 빨라집니다. 선행연구는 세 가지 분야가 존재하며 각 분야의 선행연구 효과는 중첩할 수 있습니다.\n\n선행연구는 약물과 같은 방식으로 작동하지만 부작용이 존재하지 않으며, 중첩할수록 눈에 띄는 효과를 보입니다.</t>
+  </si>
+  <si>
     <t>RecipeDef+ResearchPapersRecipe.label</t>
   </si>
   <si>
@@ -239,6 +343,9 @@
     <t>Write Research Papers</t>
   </si>
   <si>
+    <t>연구자료 작성</t>
+  </si>
+  <si>
     <t>RecipeDef+ResearchPapersRecipe.description</t>
   </si>
   <si>
@@ -248,6 +355,9 @@
     <t>Research Papers are used for simple research and is written by examining one of the 3 basic research samples.\n\nResearch papers last 24 hours when doing simple research.</t>
   </si>
   <si>
+    <t>기초적인 연구에 사용됩니다. 3가지 표본 중 하나를 연구하여 작성할 수 있습니다.\n\n24시간 동안 기초적인 연구가 가능합니다.</t>
+  </si>
+  <si>
     <t>RecipeDef+ResearchPapersRecipe.jobString</t>
   </si>
   <si>
@@ -257,6 +367,9 @@
     <t>Writing Research Papers.</t>
   </si>
   <si>
+    <t>연구자료 작성 중</t>
+  </si>
+  <si>
     <t>RecipeDef+ResearchDataRecipe.label</t>
   </si>
   <si>
@@ -266,6 +379,9 @@
     <t>Assemble Research Data</t>
   </si>
   <si>
+    <t>첨단 연구자료 제작</t>
+  </si>
+  <si>
     <t>RecipeDef+ResearchDataRecipe.description</t>
   </si>
   <si>
@@ -275,6 +391,9 @@
     <t>Research Data are used for high-tech research and is Assemble with steel, silver and all 3 basic research samples.\n\nResearch data last 24 hours when doing high-tech research.</t>
   </si>
   <si>
+    <t>첨단 연구에 사용됩니다. 강철, 은 그리고 3가지 표본을 연구하여 제작할 수 있습니다.\n\n24시간 동안 첨단 연구가 가능합니다.</t>
+  </si>
+  <si>
     <t>RecipeDef+ResearchDataRecipe.jobString</t>
   </si>
   <si>
@@ -284,6 +403,9 @@
     <t>Assembling Research Data.</t>
   </si>
   <si>
+    <t>첨단 연구자료 제작 중</t>
+  </si>
+  <si>
     <t>RecipeDef+AnalyzerDataRecipe.label</t>
   </si>
   <si>
@@ -293,6 +415,9 @@
     <t>Assemble Analyzer Data</t>
   </si>
   <si>
+    <t>암호화 연구자료 제작</t>
+  </si>
+  <si>
     <t>RecipeDef+AnalyzerDataRecipe.description</t>
   </si>
   <si>
@@ -302,6 +427,9 @@
     <t>Analyzer Data are required for the multi-analyzer to function. Its expansive, and use gold and all 4 types og research samples.\n\nAnalyzer Data last 3 days when being researched at the multi-analyzer.</t>
   </si>
   <si>
+    <t>복합 분석기가 필요한 연구에 사용됩니다. 금과 4가지 표본을 연구하여 제작할 수 있습니다.\n\n3일간 복합 분석기를 가동할 수 있습니다.</t>
+  </si>
+  <si>
     <t>RecipeDef+AnalyzerDataRecipe.jobString</t>
   </si>
   <si>
@@ -311,6 +439,9 @@
     <t>Assembling Analyzer Data.</t>
   </si>
   <si>
+    <t>암호화 연구자료 제작 중</t>
+  </si>
+  <si>
     <t>RecipeDef+ArchotechDataRecipe.label</t>
   </si>
   <si>
@@ -320,6 +451,9 @@
     <t>Extract Archotech Data</t>
   </si>
   <si>
+    <t>초월공학 연구자료 추출</t>
+  </si>
+  <si>
     <t>RecipeDef+ArchotechDataRecipe.description</t>
   </si>
   <si>
@@ -329,6 +463,9 @@
     <t>Archotech data can only be found, rewarded, or extracted from rare artifacts. Archotech data are required for the archotech analyzer to function when doing research.\n\nArchotech data last 3 days when being researched at the archotech analyzer.</t>
   </si>
   <si>
+    <t>초월공학 분석기가 필요한 연구에 사용됩니다. 임무 보상, 발견, 혹은 유물에서 추출하여 획득할 수 있습니다.\n\n3일간 초월공학 분석기를 가동할 수 있습니다.</t>
+  </si>
+  <si>
     <t>RecipeDef+ArchotechDataRecipe.jobString</t>
   </si>
   <si>
@@ -338,6 +475,9 @@
     <t>Extracting Archotech Data.</t>
   </si>
   <si>
+    <t>초월공학 연구자료 추출 중</t>
+  </si>
+  <si>
     <t>RecipeDef+OrganicResearchSamplesRecipe.label</t>
   </si>
   <si>
@@ -347,6 +487,9 @@
     <t>Collect Organic Research Samples</t>
   </si>
   <si>
+    <t>유기물 표본 수집</t>
+  </si>
+  <si>
     <t>RecipeDef+OrganicResearchSamplesRecipe.description</t>
   </si>
   <si>
@@ -356,6 +499,9 @@
     <t>Organic research samples are collected from organic nutrition, to use and examined when writing research papers or assembling research data.</t>
   </si>
   <si>
+    <t>유기물에서 수집한 표본입니다. 연구자료 작성 및 제작에 사용됩니다.</t>
+  </si>
+  <si>
     <t>RecipeDef+OrganicResearchSamplesRecipe.jobString</t>
   </si>
   <si>
@@ -374,6 +520,9 @@
     <t>Collect Metallic Research Samples</t>
   </si>
   <si>
+    <t>금속 표본 수집</t>
+  </si>
+  <si>
     <t>RecipeDef+MetallicResearchSamplesRecipe.description</t>
   </si>
   <si>
@@ -383,6 +532,9 @@
     <t>Metallic research samples are collected from metallic resources, to use and examined when writing research papers or assembling research data.</t>
   </si>
   <si>
+    <t>금속에서 수집한 표본입니다. 연구자료 작성 및 제작에 사용됩니다.</t>
+  </si>
+  <si>
     <t>RecipeDef+MetallicResearchSamplesRecipe.jobString</t>
   </si>
   <si>
@@ -392,6 +544,9 @@
     <t>Collecting Metallic Research Samples.</t>
   </si>
   <si>
+    <t>금속 표본 수집 중</t>
+  </si>
+  <si>
     <t>RecipeDef+FabricResearchSamplesRecipe.label</t>
   </si>
   <si>
@@ -401,6 +556,9 @@
     <t>Collect Fabric Research Samples</t>
   </si>
   <si>
+    <t>섬유 표본 수집</t>
+  </si>
+  <si>
     <t>RecipeDef+FabricResearchSamplesRecipe.description</t>
   </si>
   <si>
@@ -410,6 +568,9 @@
     <t>Fabric research samples are collected from cloth and leather fabrics, to use and examined when writing research papers or assembling research data.</t>
   </si>
   <si>
+    <t>섬유에서 수집한 표본입니다. 연구자료 작성 및 제작에 사용됩니다.</t>
+  </si>
+  <si>
     <t>RecipeDef+FabricResearchSamplesRecipe.jobString</t>
   </si>
   <si>
@@ -419,6 +580,9 @@
     <t>Collecting Fabric Research Samples.</t>
   </si>
   <si>
+    <t>섬유 표본 수집 중</t>
+  </si>
+  <si>
     <t>RecipeDef+ComponentResearchSamplesRecipe.label</t>
   </si>
   <si>
@@ -428,6 +592,9 @@
     <t>Collect Component Research Samples</t>
   </si>
   <si>
+    <t>부품 표본 수집</t>
+  </si>
+  <si>
     <t>RecipeDef+ComponentResearchSamplesRecipe.description</t>
   </si>
   <si>
@@ -437,6 +604,9 @@
     <t>Component research samples are collected from Industrial components, to use and examined when assembling research data.</t>
   </si>
   <si>
+    <t>부품에서 수집한 표본입니다. 고급 연구자료 제작에 사용됩니다.</t>
+  </si>
+  <si>
     <t>RecipeDef+ComponentResearchSamplesRecipe.jobString</t>
   </si>
   <si>
@@ -446,6 +616,9 @@
     <t>Collecting Component Research Samples.</t>
   </si>
   <si>
+    <t>부품 표본 수집 중</t>
+  </si>
+  <si>
     <t>RecipeDef+OrganicResearchSamplesExpertRecipe.label</t>
   </si>
   <si>
@@ -455,6 +628,9 @@
     <t>Expert - Collect Organic Research Samples x2</t>
   </si>
   <si>
+    <t>유기물 표본 수집 x2</t>
+  </si>
+  <si>
     <t>RecipeDef+OrganicResearchSamplesExpertRecipe.description</t>
   </si>
   <si>
@@ -470,6 +646,9 @@
     <t>OrganicResearchSamplesExpertRecipe.jobString</t>
   </si>
   <si>
+    <t>유기물 표본 수집 중</t>
+  </si>
+  <si>
     <t>RecipeDef+MetallicResearchSamplesExpertRecipe.label</t>
   </si>
   <si>
@@ -479,6 +658,9 @@
     <t>Expert - Collect Metallic Research Samples x2</t>
   </si>
   <si>
+    <t>금속 표본 수집 x2</t>
+  </si>
+  <si>
     <t>RecipeDef+MetallicResearchSamplesExpertRecipe.description</t>
   </si>
   <si>
@@ -500,6 +682,9 @@
     <t>Expert - Collect Fabric Research Samples x2</t>
   </si>
   <si>
+    <t>섬유 표본 수집 x2</t>
+  </si>
+  <si>
     <t>RecipeDef+FabricResearchSamplesExpertRecipe.description</t>
   </si>
   <si>
@@ -524,6 +709,18 @@
     <t>RecipeDef+ComponentResearchSamplesExpertRecipe.description</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>부품 표본 수집 x2</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>ComponentResearchSamplesExpertRecipe.description</t>
   </si>
   <si>
@@ -542,6 +739,9 @@
     <t>Make Biology Schematics</t>
   </si>
   <si>
+    <t>자연과학 선행연구 정리</t>
+  </si>
+  <si>
     <t>RecipeDef+BiologySchematicsRecipe.description</t>
   </si>
   <si>
@@ -557,6 +757,9 @@
     <t>Makeing Biology Schematics.</t>
   </si>
   <si>
+    <t>자연과학 선행연구 정리하는 중</t>
+  </si>
+  <si>
     <t>RecipeDef+ClinicalSchematicsRecipe.label</t>
   </si>
   <si>
@@ -566,6 +769,9 @@
     <t>Make Clinical Schematics</t>
   </si>
   <si>
+    <t>수리과학 선행연구 정리</t>
+  </si>
+  <si>
     <t>RecipeDef+ClinicalSchematicsRecipe.description</t>
   </si>
   <si>
@@ -581,6 +787,9 @@
     <t>Makeing Clinical Schematics.</t>
   </si>
   <si>
+    <t>수리과학 선행연구 정리하는 중</t>
+  </si>
+  <si>
     <t>RecipeDef+EngineeringSchematicsRecipe.label</t>
   </si>
   <si>
@@ -590,6 +799,9 @@
     <t>Make Engineering Schematics</t>
   </si>
   <si>
+    <t>응용과학 선행연구 정리</t>
+  </si>
+  <si>
     <t>RecipeDef+EngineeringSchematicsRecipe.description</t>
   </si>
   <si>
@@ -605,6 +817,9 @@
     <t>Makeing Engineering Schematics.</t>
   </si>
   <si>
+    <t>응용과학 선행연구 정리하는 중</t>
+  </si>
+  <si>
     <t>ThingDef+ResearchPapers.label</t>
   </si>
   <si>
@@ -614,6 +829,9 @@
     <t>Research Papers</t>
   </si>
   <si>
+    <t>연구자료</t>
+  </si>
+  <si>
     <t>ThingDef+ResearchPapers.description</t>
   </si>
   <si>
@@ -629,6 +847,9 @@
     <t>Research Data</t>
   </si>
   <si>
+    <t>첨단 연구자료</t>
+  </si>
+  <si>
     <t>ThingDef+ResearchData.description</t>
   </si>
   <si>
@@ -644,6 +865,9 @@
     <t>Analyzer Data</t>
   </si>
   <si>
+    <t>암호화 연구자료</t>
+  </si>
+  <si>
     <t>ThingDef+AnalyzerData.description</t>
   </si>
   <si>
@@ -659,6 +883,9 @@
     <t>Archotech Data</t>
   </si>
   <si>
+    <t>초월공학 연구자료</t>
+  </si>
+  <si>
     <t>ThingDef+ArchotechData.description</t>
   </si>
   <si>
@@ -674,6 +901,9 @@
     <t>Organic Research Samples</t>
   </si>
   <si>
+    <t>유기물 표본</t>
+  </si>
+  <si>
     <t>ThingDef+OrganicResearchSamples.description</t>
   </si>
   <si>
@@ -689,6 +919,9 @@
     <t>Metallic Research Samples</t>
   </si>
   <si>
+    <t>금속 표본</t>
+  </si>
+  <si>
     <t>ThingDef+MetallicResearchSamples.description</t>
   </si>
   <si>
@@ -704,6 +937,9 @@
     <t>Fabric Research Samples</t>
   </si>
   <si>
+    <t>섬유 표본</t>
+  </si>
+  <si>
     <t>ThingDef+FabricResearchSamples.description</t>
   </si>
   <si>
@@ -719,6 +955,9 @@
     <t>Component Research Samples</t>
   </si>
   <si>
+    <t>부품 표본</t>
+  </si>
+  <si>
     <t>ThingDef+ComponentResearchSamples.description</t>
   </si>
   <si>
@@ -746,6 +985,9 @@
     <t>Samples</t>
   </si>
   <si>
+    <t>표본</t>
+  </si>
+  <si>
     <t>ThingCategoryDef+Schematics.label</t>
   </si>
   <si>
@@ -755,6 +997,9 @@
     <t>Schematics</t>
   </si>
   <si>
+    <t>선행연구</t>
+  </si>
+  <si>
     <t>ThingDef+ResearchSampleBench.label</t>
   </si>
   <si>
@@ -764,6 +1009,9 @@
     <t>Research Sample Bench</t>
   </si>
   <si>
+    <t>표본 작업대</t>
+  </si>
+  <si>
     <t>ThingDef+ResearchSampleBench.description</t>
   </si>
   <si>
@@ -773,6 +1021,9 @@
     <t>The research samples bench is used to collect research samples to write research papers and assemble research data that is needed to do any research. Links to research benches: +10% research bonus.</t>
   </si>
   <si>
+    <t>표본 수집과 연구자료 작성 및 제작에 사용되는 작업대입니다. 연구대 근처에 부착되면 연구 속도를 올려줍니다.</t>
+  </si>
+  <si>
     <t>ThingDef+ArchotechAnalyzer.label</t>
   </si>
   <si>
@@ -782,6 +1033,9 @@
     <t>Archotech Analyzer</t>
   </si>
   <si>
+    <t>초월공학 분석기</t>
+  </si>
+  <si>
     <t>ThingDef+ArchotechAnalyzer.description</t>
   </si>
   <si>
@@ -791,6 +1045,9 @@
     <t>The Archotech Analyzer is a very high-tech reconstruction of the Analyzer modul, combind with archotech data. It uses Archotech Data when build and to function, constantly use data at all time, giving a huge +50% resourch bonus when active.</t>
   </si>
   <si>
+    <t>초월공학 연구자료를 사용해 재설계한 복합 분석기입니다. 제작 시 초월공학 연구자료가 필요합니다. 연구대 근처에 부착되면 연구 속도를 올려줍니다.</t>
+  </si>
+  <si>
     <t>ThingDef+ArchotechAnalyzer.comps.3.fuelLabel</t>
   </si>
   <si>
@@ -809,6 +1066,9 @@
     <t>craft</t>
   </si>
   <si>
+    <t>제작</t>
+  </si>
+  <si>
     <t>WorkGiverDef+DoResearchSampleBench.verb</t>
   </si>
   <si>
@@ -827,222 +1087,102 @@
     <t>Crafting at</t>
   </si>
   <si>
+    <t>에서 제작</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>ThingDef</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>ThingDef+SimpleResearchBench.comps.2.fuelLabel</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>SimpleResearchBench.comps.2.fuelLabel</t>
   </si>
   <si>
     <t>MultiAnalyzer.comps.3.fuelLabel</t>
   </si>
   <si>
-    <t>에서 제작</t>
-  </si>
-  <si>
-    <t>제작</t>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>ThingDef+HiTechResearchBench.comps.4.fuelLabel</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>HiTechResearchBench.comps.4.fuelLabel</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>ThingDef+MultiAnalyzer.comps.3.fuelLabel</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <t>Patches.ThingDef+SimpleResearchBench.comps.1.fuelLabel</t>
+  </si>
+  <si>
+    <t>Patches.ThingDef</t>
+  </si>
+  <si>
+    <t>SimpleResearchBench.comps.1.fuelLabel</t>
+  </si>
+  <si>
+    <t>Patches.ThingDef+HiTechResearchBench.comps.4.fuelLabel</t>
+  </si>
+  <si>
+    <t>HiTechResearchBench.comps.4.fuelLabel</t>
+  </si>
+  <si>
+    <t>Patches.ThingDef+MultiAnalyzer.comps.3.fuelLabel</t>
+  </si>
+  <si>
+    <t>연구자료</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>첨단 연구자료</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>암호화 연구자료</t>
-  </si>
-  <si>
-    <t>연구자료</t>
-  </si>
-  <si>
-    <t>첨단 연구자료</t>
-  </si>
-  <si>
-    <t>초월공학 연구자료</t>
-  </si>
-  <si>
-    <t>초월공학 연구자료를 사용해 재설계한 복합 분석기입니다. 제작 시 초월공학 연구자료가 필요합니다. 연구대 근처에 부착되면 연구 속도를 올려줍니다.</t>
-  </si>
-  <si>
-    <t>초월공학 분석기</t>
-  </si>
-  <si>
-    <t>표본 수집과 연구자료 작성 및 제작에 사용되는 작업대입니다. 연구대 근처에 부착되면 연구 속도를 올려줍니다.</t>
-  </si>
-  <si>
-    <t>표본 작업대</t>
-  </si>
-  <si>
-    <t>부품에서 수집한 표본입니다. 고급 연구자료 제작에 사용됩니다.</t>
-  </si>
-  <si>
-    <t>부품 표본</t>
-  </si>
-  <si>
-    <t>섬유에서 수집한 표본입니다. 연구자료 작성 및 제작에 사용됩니다.</t>
-  </si>
-  <si>
-    <t>섬유 표본</t>
-  </si>
-  <si>
-    <t>금속에서 수집한 표본입니다. 연구자료 작성 및 제작에 사용됩니다.</t>
-  </si>
-  <si>
-    <t>금속 표본</t>
-  </si>
-  <si>
-    <t>유기물에서 수집한 표본입니다. 연구자료 작성 및 제작에 사용됩니다.</t>
-  </si>
-  <si>
-    <t>유기물 표본</t>
-  </si>
-  <si>
-    <t>초월공학 분석기가 필요한 연구에 사용됩니다. 임무 보상, 발견, 혹은 유물에서 추출하여 획득할 수 있습니다.\n\n3일간 초월공학 분석기를 가동할 수 있습니다.</t>
-  </si>
-  <si>
-    <t>복합 분석기가 필요한 연구에 사용됩니다. 금과 4가지 표본을 연구하여 제작할 수 있습니다.\n\n3일간 복합 분석기를 가동할 수 있습니다.</t>
-  </si>
-  <si>
-    <t>첨단 연구에 사용됩니다. 강철, 은 그리고 3가지 표본을 연구하여 제작할 수 있습니다.\n\n24시간 동안 첨단 연구가 가능합니다.</t>
-  </si>
-  <si>
-    <t>기초적인 연구에 사용됩니다. 3가지 표본 중 하나를 연구하여 작성할 수 있습니다.\n\n24시간 동안 기초적인 연구가 가능합니다.</t>
-  </si>
-  <si>
-    <t>사용 시 앞선 연구자들의 응용과학 선행연구를 검토하여 연구 진척이 빨라집니다. 선행연구는 세 가지 분야가 존재하며 각 분야의 선행연구 효과는 중첩할 수 있습니다.\n\n선행연구는 약물과 같은 방식으로 작동하지만 부작용이 존재하지 않으며, 중첩할수록 눈에 띄는 효과를 보입니다.</t>
-  </si>
-  <si>
-    <t>응용과학 선행연구</t>
-  </si>
-  <si>
-    <t>{0} 검토하는 중</t>
-  </si>
-  <si>
-    <t>{0} 검토하기</t>
-  </si>
-  <si>
-    <t>사용 시 앞선 연구자들의 수리과학 선행연구를 검토하여 연구 진척이 빨라집니다. 선행연구는 세 가지 분야가 존재하며 각 분야의 선행연구 효과는 중첩할 수 있습니다.\n\n선행연구는 약물과 같은 방식으로 작동하지만 부작용이 존재하지 않으며, 중첩할수록 눈에 띄는 효과를 보입니다.</t>
-  </si>
-  <si>
-    <t>수리과학 선행연구</t>
-  </si>
-  <si>
-    <t>사용 시 앞선 연구자들의 자연과학 선행연구를 검토하여 연구 진척이 빨라집니다. 선행연구는 세 가지 분야가 존재하며 각 분야의 선행연구 효과는 중첩할 수 있습니다.\n\n선행연구는 약물과 같은 방식으로 작동하지만 부작용이 존재하지 않으며, 중첩할수록 눈에 띄는 효과를 보입니다.</t>
-  </si>
-  <si>
-    <t>자연과학 선행연구</t>
-  </si>
-  <si>
-    <t>선행연구</t>
-  </si>
-  <si>
-    <t>표본</t>
-  </si>
-  <si>
-    <t>응용과학 선행연구 정리하는 중</t>
-  </si>
-  <si>
-    <t>응용과학 선행연구 정리</t>
-  </si>
-  <si>
-    <t>수리과학 선행연구 정리하는 중</t>
-  </si>
-  <si>
-    <t>수리과학 선행연구 정리</t>
-  </si>
-  <si>
-    <t>자연과학 선행연구 정리하는 중</t>
-  </si>
-  <si>
-    <t>자연과학 선행연구 정리</t>
-  </si>
-  <si>
-    <t>부품 표본 수집 중</t>
-  </si>
-  <si>
-    <t>섬유 표본 수집 x2</t>
-  </si>
-  <si>
-    <t>섬유 표본 수집 중</t>
-  </si>
-  <si>
-    <t>금속 표본 수집 중</t>
-  </si>
-  <si>
-    <t>금속 표본 수집 x2</t>
-  </si>
-  <si>
-    <t>유기물 표본 수집 중</t>
-  </si>
-  <si>
-    <t>유기물 표본 수집 x2</t>
-  </si>
-  <si>
-    <t>부품 표본 수집</t>
-  </si>
-  <si>
-    <t>섬유 표본 수집</t>
-  </si>
-  <si>
-    <t>금속 표본 수집</t>
-  </si>
-  <si>
-    <t>유기물 표본 수집</t>
-  </si>
-  <si>
-    <t>초월공학 연구자료 추출 중</t>
-  </si>
-  <si>
-    <t>초월공학 연구자료 추출</t>
-  </si>
-  <si>
-    <t>암호화 연구자료 제작 중</t>
-  </si>
-  <si>
-    <t>암호화 연구자료 제작</t>
-  </si>
-  <si>
-    <t>첨단 연구자료 제작 중</t>
-  </si>
-  <si>
-    <t>첨단 연구자료 제작</t>
-  </si>
-  <si>
-    <t>연구자료 작성 중</t>
-  </si>
-  <si>
-    <t>연구자료 작성</t>
-  </si>
-  <si>
-    <t>앞선 연구자들의 응용과학 선행연구를 검토하여 연구 진척이 빨라집니다. 선행연구는 세 가지 분야가 존재하며 각 분야의 선행연구 효과는 중첩할 수 있습니다.\n\n선행연구는 약물과 같은 방식으로 작동하지만 부작용이 존재하지 않으며, 중첩할수록 눈에 띄는 효과를 보입니다.</t>
-  </si>
-  <si>
-    <t>응용과학 선행연구 검토</t>
-  </si>
-  <si>
-    <t>앞선 연구자들의 수리과학 선행연구를 검토하여 연구 진척이 빨라집니다. 선행연구는 세 가지 분야가 존재하며 각 분야의 선행연구 효과는 중첩할 수 있습니다.\n\n선행연구는 약물과 같은 방식으로 작동하지만 부작용이 존재하지 않으며, 중첩할수록 눈에 띄는 효과를 보입니다.</t>
-  </si>
-  <si>
-    <t>수리과학 선행연구 검토</t>
-  </si>
-  <si>
-    <t>앞선 연구자들의 자연과학 선행연구를 검토하여 연구 진척이 빨라집니다. 선행연구는 세 가지 분야가 존재하며 각 분야의 선행연구 효과는 중첩할 수 있습니다.\n\n선행연구는 약물과 같은 방식으로 작동하지만 부작용이 존재하지 않으며, 중첩할수록 눈에 띄는 효과를 보입니다.</t>
-  </si>
-  <si>
-    <t>자연과학 선행연구 검토</t>
-  </si>
-  <si>
-    <t>ThingDef+SimpleResearchBench.comps.2.fuelLabel</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>ThingDef+MultiAnalyzer.comps.3.fuelLabel</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>ThingDef</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>부품 표본 수집 x2</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>HiTechResearchBench.comps.4.fuelLabel</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>ThingDef+HiTechResearchBench.comps.4.fuelLabel</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -1050,7 +1190,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1069,13 +1209,29 @@
       <family val="3"/>
       <charset val="129"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF87CEEB"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -1090,9 +1246,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyBorder="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
@@ -1394,11 +1552,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F97"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A54" workbookViewId="0">
-      <selection activeCell="D69" sqref="D69"/>
+    <sheetView tabSelected="1" topLeftCell="A84" workbookViewId="0">
+      <selection activeCell="F100" sqref="F100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="17" x14ac:dyDescent="0.45"/>
@@ -1409,7 +1567,8 @@
     <col min="4" max="4" width="29.26953125" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="42.54296875" style="1" customWidth="1"/>
     <col min="6" max="6" width="31.453125" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.1796875" style="1"/>
+    <col min="7" max="7" width="9.1796875" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.1796875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.45">
@@ -1446,1571 +1605,1571 @@
         <v>9</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>295</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>294</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>291</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A5" s="1" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>290</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A6" s="1" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>328</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A7" s="1" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>328</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A8" s="1" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>327</v>
+        <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A9" s="1" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>293</v>
+        <v>37</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A10" s="1" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>292</v>
+        <v>41</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A11" s="1" t="s">
-        <v>34</v>
+        <v>42</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>291</v>
+        <v>18</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A12" s="1" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>290</v>
+        <v>22</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A13" s="1" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>326</v>
+        <v>49</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A14" s="1" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>326</v>
+        <v>49</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A15" s="1" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>45</v>
+        <v>54</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>325</v>
+        <v>55</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A16" s="1" t="s">
-        <v>46</v>
+        <v>56</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>47</v>
+        <v>57</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>48</v>
+        <v>58</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>289</v>
+        <v>59</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A17" s="1" t="s">
-        <v>49</v>
+        <v>60</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>50</v>
+        <v>61</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>51</v>
+        <v>62</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>288</v>
+        <v>63</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A18" s="1" t="s">
-        <v>52</v>
+        <v>64</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>53</v>
+        <v>65</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>291</v>
+        <v>18</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A19" s="1" t="s">
-        <v>54</v>
+        <v>66</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>55</v>
+        <v>67</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>290</v>
+        <v>22</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A20" s="1" t="s">
-        <v>56</v>
+        <v>68</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>57</v>
+        <v>69</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>58</v>
+        <v>70</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>324</v>
+        <v>71</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A21" s="1" t="s">
-        <v>59</v>
+        <v>72</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>60</v>
+        <v>73</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>61</v>
+        <v>74</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>324</v>
+        <v>71</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A22" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="E22" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="B22" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>51</v>
-      </c>
       <c r="F22" s="1" t="s">
-        <v>323</v>
+        <v>77</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A23" s="1" t="s">
-        <v>64</v>
+        <v>78</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>65</v>
+        <v>79</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>66</v>
+        <v>80</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>67</v>
+        <v>81</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>322</v>
+        <v>82</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A24" s="1" t="s">
-        <v>68</v>
+        <v>83</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>65</v>
+        <v>79</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>69</v>
+        <v>84</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>70</v>
+        <v>85</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>287</v>
+        <v>86</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A25" s="1" t="s">
-        <v>71</v>
+        <v>87</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>65</v>
+        <v>79</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>72</v>
+        <v>88</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>73</v>
+        <v>89</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>321</v>
+        <v>90</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A26" s="1" t="s">
-        <v>74</v>
+        <v>91</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>65</v>
+        <v>79</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>75</v>
+        <v>92</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>76</v>
+        <v>93</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>320</v>
+        <v>94</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A27" s="1" t="s">
-        <v>77</v>
+        <v>95</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>65</v>
+        <v>79</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>78</v>
+        <v>96</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>79</v>
+        <v>97</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>286</v>
+        <v>98</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A28" s="1" t="s">
-        <v>80</v>
+        <v>99</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>65</v>
+        <v>79</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>81</v>
+        <v>100</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>82</v>
+        <v>101</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>319</v>
+        <v>102</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A29" s="1" t="s">
-        <v>83</v>
+        <v>103</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>65</v>
+        <v>79</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>84</v>
+        <v>104</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>85</v>
+        <v>105</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>318</v>
+        <v>106</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A30" s="1" t="s">
-        <v>86</v>
+        <v>107</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>65</v>
+        <v>79</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>87</v>
+        <v>108</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>88</v>
+        <v>109</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>285</v>
+        <v>110</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A31" s="1" t="s">
-        <v>89</v>
+        <v>111</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>65</v>
+        <v>79</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>90</v>
+        <v>112</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>91</v>
+        <v>113</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>317</v>
+        <v>114</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A32" s="1" t="s">
-        <v>92</v>
+        <v>115</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>65</v>
+        <v>79</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>93</v>
+        <v>116</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>94</v>
+        <v>117</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>316</v>
+        <v>118</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A33" s="1" t="s">
-        <v>95</v>
+        <v>119</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>65</v>
+        <v>79</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>96</v>
+        <v>120</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>97</v>
+        <v>121</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>284</v>
+        <v>122</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A34" s="1" t="s">
-        <v>98</v>
+        <v>123</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>65</v>
+        <v>79</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>99</v>
+        <v>124</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>100</v>
+        <v>125</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>315</v>
+        <v>126</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A35" s="1" t="s">
-        <v>101</v>
+        <v>127</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>65</v>
+        <v>79</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>102</v>
+        <v>128</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>103</v>
+        <v>129</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>314</v>
+        <v>130</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A36" s="1" t="s">
-        <v>104</v>
+        <v>131</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>65</v>
+        <v>79</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>105</v>
+        <v>132</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>106</v>
+        <v>133</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>282</v>
+        <v>134</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A37" s="1" t="s">
-        <v>107</v>
+        <v>135</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>65</v>
+        <v>79</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>108</v>
+        <v>136</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>109</v>
+        <v>137</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>314</v>
+        <v>130</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A38" s="1" t="s">
-        <v>110</v>
+        <v>138</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>65</v>
+        <v>79</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>111</v>
+        <v>139</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>112</v>
+        <v>140</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>313</v>
+        <v>141</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A39" s="1" t="s">
-        <v>113</v>
+        <v>142</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>65</v>
+        <v>79</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>114</v>
+        <v>143</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>115</v>
+        <v>144</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>280</v>
+        <v>145</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A40" s="1" t="s">
-        <v>116</v>
+        <v>146</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>65</v>
+        <v>79</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>117</v>
+        <v>147</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>118</v>
+        <v>148</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>307</v>
+        <v>149</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A41" s="1" t="s">
-        <v>119</v>
+        <v>150</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>65</v>
+        <v>79</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>120</v>
+        <v>151</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>121</v>
+        <v>152</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>312</v>
+        <v>153</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A42" s="1" t="s">
-        <v>122</v>
+        <v>154</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>65</v>
+        <v>79</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>123</v>
+        <v>155</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>124</v>
+        <v>156</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>278</v>
+        <v>157</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A43" s="1" t="s">
-        <v>125</v>
+        <v>158</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>65</v>
+        <v>79</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>126</v>
+        <v>159</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>127</v>
+        <v>160</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>306</v>
+        <v>161</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A44" s="1" t="s">
-        <v>128</v>
+        <v>162</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>65</v>
+        <v>79</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>129</v>
+        <v>163</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>130</v>
+        <v>164</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>311</v>
+        <v>165</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A45" s="1" t="s">
-        <v>131</v>
+        <v>166</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>65</v>
+        <v>79</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>132</v>
+        <v>167</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>133</v>
+        <v>168</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>276</v>
+        <v>169</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A46" s="1" t="s">
-        <v>134</v>
+        <v>170</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>65</v>
+        <v>79</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>135</v>
+        <v>171</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>136</v>
+        <v>172</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>304</v>
+        <v>173</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A47" s="1" t="s">
-        <v>137</v>
+        <v>174</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>65</v>
+        <v>79</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>138</v>
+        <v>175</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>139</v>
+        <v>176</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>310</v>
+        <v>177</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A48" s="1" t="s">
-        <v>140</v>
+        <v>178</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>65</v>
+        <v>79</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>141</v>
+        <v>179</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>142</v>
+        <v>180</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>282</v>
+        <v>134</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A49" s="1" t="s">
-        <v>143</v>
+        <v>181</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>65</v>
+        <v>79</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>144</v>
+        <v>182</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>109</v>
+        <v>137</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>309</v>
+        <v>183</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A50" s="1" t="s">
-        <v>145</v>
+        <v>184</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>65</v>
+        <v>79</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>146</v>
+        <v>185</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>147</v>
+        <v>186</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>308</v>
+        <v>187</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A51" s="1" t="s">
-        <v>148</v>
+        <v>188</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>65</v>
+        <v>79</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>149</v>
+        <v>189</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>115</v>
+        <v>144</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>280</v>
+        <v>145</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A52" s="1" t="s">
-        <v>150</v>
+        <v>190</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>65</v>
+        <v>79</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>151</v>
+        <v>191</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>118</v>
+        <v>148</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>307</v>
+        <v>149</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A53" s="1" t="s">
-        <v>152</v>
+        <v>192</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>65</v>
+        <v>79</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>153</v>
+        <v>193</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>154</v>
+        <v>194</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>305</v>
+        <v>195</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A54" s="1" t="s">
-        <v>155</v>
+        <v>196</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>65</v>
+        <v>79</v>
       </c>
       <c r="C54" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="E54" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="E54" s="1" t="s">
-        <v>124</v>
-      </c>
       <c r="F54" s="1" t="s">
-        <v>278</v>
+        <v>157</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A55" s="1" t="s">
-        <v>157</v>
+        <v>198</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>65</v>
+        <v>79</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>158</v>
+        <v>199</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>127</v>
+        <v>160</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>306</v>
+        <v>161</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A56" s="1" t="s">
-        <v>159</v>
+        <v>200</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>65</v>
+        <v>79</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>160</v>
+        <v>201</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>161</v>
+        <v>202</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>332</v>
+        <v>204</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A57" s="1" t="s">
-        <v>162</v>
+        <v>203</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>65</v>
+        <v>79</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>163</v>
+        <v>205</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>133</v>
+        <v>168</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>276</v>
+        <v>169</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A58" s="1" t="s">
-        <v>164</v>
+        <v>206</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>65</v>
+        <v>79</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>165</v>
+        <v>207</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>136</v>
+        <v>172</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>304</v>
+        <v>173</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A59" s="1" t="s">
-        <v>166</v>
+        <v>208</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>65</v>
+        <v>79</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>167</v>
+        <v>209</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>168</v>
+        <v>210</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>303</v>
+        <v>211</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A60" s="1" t="s">
-        <v>169</v>
+        <v>212</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>65</v>
+        <v>79</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>170</v>
+        <v>213</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>294</v>
+        <v>14</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A61" s="1" t="s">
-        <v>171</v>
+        <v>214</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>65</v>
+        <v>79</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>172</v>
+        <v>215</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>173</v>
+        <v>216</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>302</v>
+        <v>217</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A62" s="1" t="s">
-        <v>174</v>
+        <v>218</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>65</v>
+        <v>79</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>175</v>
+        <v>219</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>176</v>
+        <v>220</v>
       </c>
       <c r="F62" s="1" t="s">
-        <v>301</v>
+        <v>221</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A63" s="1" t="s">
-        <v>177</v>
+        <v>222</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>65</v>
+        <v>79</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>178</v>
+        <v>223</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="F63" s="1" t="s">
-        <v>292</v>
+        <v>41</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A64" s="1" t="s">
-        <v>179</v>
+        <v>224</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>65</v>
+        <v>79</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>180</v>
+        <v>225</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>181</v>
+        <v>226</v>
       </c>
       <c r="F64" s="1" t="s">
-        <v>300</v>
+        <v>227</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A65" s="1" t="s">
-        <v>182</v>
+        <v>228</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>65</v>
+        <v>79</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>183</v>
+        <v>229</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>184</v>
+        <v>230</v>
       </c>
       <c r="F65" s="1" t="s">
-        <v>299</v>
+        <v>231</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A66" s="1" t="s">
-        <v>185</v>
+        <v>232</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>65</v>
+        <v>79</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>186</v>
+        <v>233</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>51</v>
+        <v>62</v>
       </c>
       <c r="F66" s="1" t="s">
-        <v>288</v>
+        <v>63</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A67" s="1" t="s">
-        <v>187</v>
+        <v>234</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>65</v>
+        <v>79</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>188</v>
+        <v>235</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>189</v>
+        <v>236</v>
       </c>
       <c r="F67" s="1" t="s">
-        <v>298</v>
+        <v>237</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A68" s="1" t="s">
-        <v>190</v>
+        <v>238</v>
       </c>
       <c r="B68" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>191</v>
+        <v>239</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>192</v>
+        <v>240</v>
       </c>
       <c r="F68" s="1" t="s">
-        <v>269</v>
+        <v>241</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A69" s="1" t="s">
-        <v>193</v>
+        <v>242</v>
       </c>
       <c r="B69" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>194</v>
+        <v>243</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>70</v>
+        <v>85</v>
       </c>
       <c r="F69" s="1" t="s">
-        <v>287</v>
+        <v>86</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A70" s="1" t="s">
-        <v>195</v>
+        <v>244</v>
       </c>
       <c r="B70" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>196</v>
+        <v>245</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>197</v>
+        <v>246</v>
       </c>
       <c r="F70" s="1" t="s">
-        <v>270</v>
+        <v>247</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A71" s="1" t="s">
-        <v>198</v>
+        <v>248</v>
       </c>
       <c r="B71" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>199</v>
+        <v>249</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>79</v>
+        <v>97</v>
       </c>
       <c r="F71" s="1" t="s">
-        <v>286</v>
+        <v>98</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A72" s="1" t="s">
-        <v>200</v>
+        <v>250</v>
       </c>
       <c r="B72" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>201</v>
+        <v>251</v>
       </c>
       <c r="E72" s="1" t="s">
-        <v>202</v>
+        <v>252</v>
       </c>
       <c r="F72" s="1" t="s">
-        <v>268</v>
+        <v>253</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A73" s="1" t="s">
-        <v>203</v>
+        <v>254</v>
       </c>
       <c r="B73" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>204</v>
+        <v>255</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>88</v>
+        <v>109</v>
       </c>
       <c r="F73" s="1" t="s">
-        <v>285</v>
+        <v>110</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A74" s="1" t="s">
-        <v>205</v>
+        <v>256</v>
       </c>
       <c r="B74" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>206</v>
+        <v>257</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>207</v>
+        <v>258</v>
       </c>
       <c r="F74" s="1" t="s">
-        <v>271</v>
+        <v>259</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A75" s="1" t="s">
-        <v>208</v>
+        <v>260</v>
       </c>
       <c r="B75" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>209</v>
+        <v>261</v>
       </c>
       <c r="E75" s="1" t="s">
-        <v>97</v>
+        <v>121</v>
       </c>
       <c r="F75" s="1" t="s">
-        <v>284</v>
+        <v>122</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A76" s="1" t="s">
-        <v>210</v>
+        <v>262</v>
       </c>
       <c r="B76" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>211</v>
+        <v>263</v>
       </c>
       <c r="E76" s="1" t="s">
-        <v>212</v>
+        <v>264</v>
       </c>
       <c r="F76" s="1" t="s">
-        <v>283</v>
+        <v>265</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A77" s="1" t="s">
-        <v>213</v>
+        <v>266</v>
       </c>
       <c r="B77" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>214</v>
+        <v>267</v>
       </c>
       <c r="E77" s="1" t="s">
-        <v>106</v>
+        <v>133</v>
       </c>
       <c r="F77" s="1" t="s">
-        <v>282</v>
+        <v>134</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A78" s="1" t="s">
-        <v>215</v>
+        <v>268</v>
       </c>
       <c r="B78" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>216</v>
+        <v>269</v>
       </c>
       <c r="E78" s="1" t="s">
-        <v>217</v>
+        <v>270</v>
       </c>
       <c r="F78" s="1" t="s">
-        <v>281</v>
+        <v>271</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A79" s="1" t="s">
-        <v>218</v>
+        <v>272</v>
       </c>
       <c r="B79" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>219</v>
+        <v>273</v>
       </c>
       <c r="E79" s="1" t="s">
-        <v>115</v>
+        <v>144</v>
       </c>
       <c r="F79" s="1" t="s">
-        <v>280</v>
+        <v>145</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A80" s="1" t="s">
-        <v>220</v>
+        <v>274</v>
       </c>
       <c r="B80" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>221</v>
+        <v>275</v>
       </c>
       <c r="E80" s="1" t="s">
-        <v>222</v>
+        <v>276</v>
       </c>
       <c r="F80" s="1" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A81" s="1" t="s">
-        <v>223</v>
+        <v>278</v>
       </c>
       <c r="B81" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>224</v>
+        <v>279</v>
       </c>
       <c r="E81" s="1" t="s">
-        <v>124</v>
+        <v>156</v>
       </c>
       <c r="F81" s="1" t="s">
-        <v>278</v>
+        <v>157</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A82" s="1" t="s">
-        <v>225</v>
+        <v>280</v>
       </c>
       <c r="B82" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>226</v>
+        <v>281</v>
       </c>
       <c r="E82" s="1" t="s">
-        <v>227</v>
+        <v>282</v>
       </c>
       <c r="F82" s="1" t="s">
-        <v>277</v>
+        <v>283</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A83" s="1" t="s">
-        <v>228</v>
+        <v>284</v>
       </c>
       <c r="B83" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>229</v>
+        <v>285</v>
       </c>
       <c r="E83" s="1" t="s">
-        <v>133</v>
+        <v>168</v>
       </c>
       <c r="F83" s="1" t="s">
-        <v>276</v>
+        <v>169</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A84" s="1" t="s">
-        <v>230</v>
+        <v>286</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>231</v>
+        <v>287</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>232</v>
+        <v>288</v>
       </c>
       <c r="E84" s="1" t="s">
-        <v>233</v>
+        <v>289</v>
       </c>
       <c r="F84" s="1" t="s">
-        <v>269</v>
+        <v>241</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A85" s="1" t="s">
-        <v>234</v>
+        <v>290</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>231</v>
+        <v>287</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>235</v>
+        <v>291</v>
       </c>
       <c r="E85" s="1" t="s">
-        <v>236</v>
+        <v>292</v>
       </c>
       <c r="F85" s="1" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A86" s="1" t="s">
-        <v>237</v>
+        <v>294</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>231</v>
+        <v>287</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>238</v>
+        <v>295</v>
       </c>
       <c r="E86" s="1" t="s">
-        <v>239</v>
+        <v>296</v>
       </c>
       <c r="F86" s="1" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A87" s="1" t="s">
-        <v>240</v>
+        <v>298</v>
       </c>
       <c r="B87" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>241</v>
+        <v>299</v>
       </c>
       <c r="E87" s="1" t="s">
-        <v>242</v>
+        <v>300</v>
       </c>
       <c r="F87" s="1" t="s">
-        <v>275</v>
+        <v>301</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A88" s="1" t="s">
-        <v>243</v>
+        <v>302</v>
       </c>
       <c r="B88" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>244</v>
+        <v>303</v>
       </c>
       <c r="E88" s="1" t="s">
-        <v>245</v>
+        <v>304</v>
       </c>
       <c r="F88" s="1" t="s">
-        <v>274</v>
+        <v>305</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A89" s="1" t="s">
-        <v>246</v>
+        <v>306</v>
       </c>
       <c r="B89" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>247</v>
+        <v>307</v>
       </c>
       <c r="E89" s="1" t="s">
-        <v>248</v>
+        <v>308</v>
       </c>
       <c r="F89" s="1" t="s">
-        <v>273</v>
+        <v>309</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A90" s="1" t="s">
-        <v>249</v>
+        <v>310</v>
       </c>
       <c r="B90" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>250</v>
+        <v>311</v>
       </c>
       <c r="E90" s="1" t="s">
-        <v>251</v>
+        <v>312</v>
       </c>
       <c r="F90" s="1" t="s">
-        <v>272</v>
+        <v>313</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A91" s="1" t="s">
-        <v>252</v>
+        <v>314</v>
       </c>
       <c r="B91" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>253</v>
+        <v>315</v>
       </c>
       <c r="E91" s="1" t="s">
-        <v>207</v>
+        <v>258</v>
       </c>
       <c r="F91" s="1" t="s">
-        <v>271</v>
+        <v>259</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A92" s="1" t="s">
-        <v>254</v>
+        <v>316</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>255</v>
+        <v>317</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>256</v>
+        <v>318</v>
       </c>
       <c r="E92" s="1" t="s">
-        <v>257</v>
+        <v>319</v>
       </c>
       <c r="F92" s="1" t="s">
-        <v>267</v>
+        <v>320</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A93" s="1" t="s">
-        <v>258</v>
+        <v>321</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>255</v>
+        <v>317</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>259</v>
+        <v>322</v>
       </c>
       <c r="E93" s="1" t="s">
-        <v>260</v>
+        <v>323</v>
       </c>
       <c r="F93" s="1" t="s">
-        <v>267</v>
+        <v>320</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A94" s="1" t="s">
-        <v>261</v>
+        <v>324</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>255</v>
+        <v>317</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>262</v>
+        <v>325</v>
       </c>
       <c r="E94" s="1" t="s">
-        <v>263</v>
+        <v>326</v>
       </c>
       <c r="F94" s="1" t="s">
-        <v>266</v>
+        <v>327</v>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.45">
@@ -3018,54 +3177,97 @@
         <v>329</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>264</v>
-      </c>
-      <c r="E95" s="1" t="s">
-        <v>192</v>
-      </c>
-      <c r="F95" s="1" t="s">
-        <v>269</v>
+        <v>330</v>
+      </c>
+      <c r="E95" s="2" t="s">
+        <v>240</v>
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A96" s="1" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="C96" s="1" t="s">
         <v>333</v>
       </c>
-      <c r="E96" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="F96" s="1" t="s">
-        <v>270</v>
+      <c r="E96" s="2" t="s">
+        <v>246</v>
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A97" s="1" t="s">
-        <v>330</v>
+        <v>334</v>
       </c>
       <c r="B97" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="C97" s="1" t="s">
         <v>331</v>
       </c>
-      <c r="C97" s="1" t="s">
-        <v>265</v>
-      </c>
-      <c r="E97" s="1" t="s">
-        <v>202</v>
-      </c>
-      <c r="F97" s="1" t="s">
-        <v>268</v>
+      <c r="E97" s="2" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A99" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="B99" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="C99" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="E99" s="3" t="s">
+        <v>240</v>
+      </c>
+      <c r="F99" s="1" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A100" s="1" t="s">
+        <v>338</v>
+      </c>
+      <c r="B100" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="C100" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="E100" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="F100" s="1" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A101" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="B101" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="C101" s="1" t="s">
+        <v>331</v>
+      </c>
+      <c r="E101" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="F101" s="1" t="s">
+        <v>343</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>